<commit_message>
Summing the Empty Values (main v1.2)
</commit_message>
<xml_diff>
--- a/Scraped Data/Meera Industries Ltd_Data.xlsx
+++ b/Scraped Data/Meera Industries Ltd_Data.xlsx
@@ -647,6 +647,9 @@
       <c r="D5" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="E5" s="3">
+        <v>3.76</v>
+      </c>
       <c r="F5" s="3" t="s">
         <v>14</v>
       </c>
@@ -661,6 +664,9 @@
       </c>
       <c r="J5" s="3" t="s">
         <v>51</v>
+      </c>
+      <c r="K5" s="3">
+        <v>13.37</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -676,6 +682,9 @@
       <c r="D6" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="E6" s="3">
+        <v>9.040000000000001</v>
+      </c>
       <c r="F6" s="3" t="s">
         <v>15</v>
       </c>
@@ -690,6 +699,9 @@
       </c>
       <c r="J6" s="3" t="s">
         <v>52</v>
+      </c>
+      <c r="K6" s="3">
+        <v>21.89</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -705,6 +717,9 @@
       <c r="D7" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="E7" s="3">
+        <v>13.94</v>
+      </c>
       <c r="F7" s="3" t="s">
         <v>16</v>
       </c>
@@ -719,6 +734,9 @@
       </c>
       <c r="J7" s="3" t="s">
         <v>53</v>
+      </c>
+      <c r="K7" s="3">
+        <v>36.38</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -734,6 +752,9 @@
       <c r="D8" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="E8" s="3">
+        <v>23.36</v>
+      </c>
       <c r="F8" s="3" t="s">
         <v>17</v>
       </c>
@@ -748,6 +769,9 @@
       </c>
       <c r="J8" s="3" t="s">
         <v>54</v>
+      </c>
+      <c r="K8" s="3">
+        <v>21.11</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -763,6 +787,9 @@
       <c r="D9" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="E9" s="3">
+        <v>25.04</v>
+      </c>
       <c r="F9" s="3" t="s">
         <v>18</v>
       </c>
@@ -777,6 +804,9 @@
       </c>
       <c r="J9" s="3" t="s">
         <v>55</v>
+      </c>
+      <c r="K9" s="3">
+        <v>22.7</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -792,6 +822,9 @@
       <c r="D10" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="E10" s="3">
+        <v>26.15</v>
+      </c>
       <c r="F10" s="3" t="s">
         <v>19</v>
       </c>
@@ -806,6 +839,9 @@
       </c>
       <c r="J10" s="3" t="s">
         <v>56</v>
+      </c>
+      <c r="K10" s="3">
+        <v>31.89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>